<commit_message>
Code cleanups, MC6 Pro & MC8 compatibility fixes
</commit_message>
<xml_diff>
--- a/Preset CCs.xlsx
+++ b/Preset CCs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Repos\GP-MC8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DC05FB-38F6-4DBF-A3A1-B344EEC6E1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A5B6C3-990D-412E-A8D7-5238E129E7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13650" yWindow="4095" windowWidth="31500" windowHeight="15345" xr2:uid="{0B747C49-F5AE-45D7-856A-0899A5ED985A}"/>
+    <workbookView xWindow="30960" yWindow="2175" windowWidth="20445" windowHeight="12825" xr2:uid="{0B747C49-F5AE-45D7-856A-0899A5ED985A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
   <si>
     <t>A</t>
   </si>
@@ -237,6 +237,18 @@
   </si>
   <si>
     <t>Should change the 40 &amp; 41 to something else</t>
+  </si>
+  <si>
+    <t>0-3</t>
+  </si>
+  <si>
+    <t>4 &amp; 5</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>Top</t>
   </si>
 </sst>
 </file>
@@ -617,13 +629,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159D800F-0466-47B0-AEE7-B390993F0385}">
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S25" sqref="S25"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,718 +650,744 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
-      <c r="J1" s="6" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="J2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="6"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" t="s">
-        <v>54</v>
-      </c>
-      <c r="P2" t="s">
-        <v>38</v>
-      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="1">
-        <v>48</v>
-      </c>
-      <c r="G3" s="1">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="J3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>54</v>
       </c>
       <c r="P3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>18</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>30</v>
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="F5" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="Q5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1">
+        <v>50</v>
+      </c>
+      <c r="G6" s="1">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2</v>
+      </c>
+      <c r="L6" s="1">
+        <v>19</v>
+      </c>
+      <c r="P6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <v>51</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G7" s="1">
         <v>35</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F7"/>
-      <c r="P7" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F8"/>
+      <c r="P8" t="s">
         <v>61</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q8" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="1">
-        <v>52</v>
-      </c>
-      <c r="G8" s="1">
-        <v>36</v>
-      </c>
-      <c r="J8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" s="1">
-        <v>4</v>
-      </c>
-      <c r="L8" s="1">
-        <v>20</v>
-      </c>
-      <c r="P8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1">
+        <v>52</v>
+      </c>
+      <c r="G9" s="1">
+        <v>36</v>
+      </c>
+      <c r="J9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1">
-        <v>21</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="1">
-        <v>53</v>
-      </c>
-      <c r="G9" s="1">
-        <v>37</v>
-      </c>
-      <c r="J9" t="s">
-        <v>6</v>
-      </c>
       <c r="K9" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L9" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1">
+        <v>53</v>
+      </c>
+      <c r="G10" s="1">
+        <v>37</v>
+      </c>
+      <c r="J10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="1">
-        <v>22</v>
-      </c>
-      <c r="F10" s="1">
-        <v>54</v>
-      </c>
-      <c r="G10" s="1">
-        <v>38</v>
-      </c>
-      <c r="J10" t="s">
-        <v>7</v>
-      </c>
       <c r="K10" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L10" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1">
+        <v>54</v>
+      </c>
+      <c r="G11" s="1">
+        <v>38</v>
+      </c>
+      <c r="J11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="1">
+        <v>6</v>
+      </c>
+      <c r="L11" s="1">
+        <v>23</v>
+      </c>
+      <c r="P11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>7</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F12" s="1">
         <v>55</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G12" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F12"/>
-    </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1">
-        <v>24</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="1">
-        <v>56</v>
-      </c>
-      <c r="G13" s="1">
-        <v>40</v>
-      </c>
-      <c r="J13" t="s">
-        <v>8</v>
-      </c>
-      <c r="K13" s="1">
-        <v>8</v>
-      </c>
-      <c r="L13" s="1">
-        <v>24</v>
-      </c>
-      <c r="P13" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>50</v>
-      </c>
+      <c r="F13"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K14" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L14" s="1">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="P14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1">
-        <v>26</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="F15" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G15" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K15" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L15" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="1">
+        <v>58</v>
+      </c>
+      <c r="G16" s="1">
+        <v>42</v>
+      </c>
+      <c r="J16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="1">
+        <v>10</v>
+      </c>
+      <c r="L16" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <v>11</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C17" s="1">
         <v>27</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F17" s="1">
         <v>59</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G17" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F17"/>
-    </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="1">
-        <v>12</v>
-      </c>
-      <c r="C18" s="1">
-        <v>28</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="1">
-        <v>60</v>
-      </c>
-      <c r="G18" s="1">
-        <v>44</v>
-      </c>
-      <c r="J18" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="1">
-        <v>12</v>
-      </c>
-      <c r="L18" s="1">
-        <v>28</v>
-      </c>
+      <c r="F18"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F19" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G19" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J19" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="1">
         <v>12</v>
       </c>
-      <c r="K19" s="1">
-        <v>13</v>
-      </c>
       <c r="L19" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="1">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="F20" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G20" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J20" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="1">
         <v>13</v>
       </c>
-      <c r="K20" s="1">
-        <v>14</v>
-      </c>
       <c r="L20" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>14</v>
+      </c>
+      <c r="C21" s="1">
+        <v>30</v>
+      </c>
+      <c r="F21" s="1">
+        <v>62</v>
+      </c>
+      <c r="G21" s="1">
+        <v>46</v>
+      </c>
+      <c r="J21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="1">
+        <v>14</v>
+      </c>
+      <c r="L21" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="1">
         <v>15</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C22" s="1">
         <v>31</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F22" s="1">
         <v>63</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G22" s="1">
         <v>47</v>
       </c>
-      <c r="P21" s="6" t="s">
+      <c r="P22" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J23" t="s">
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
         <v>32</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="1">
-        <v>36</v>
-      </c>
-      <c r="C25" s="1">
-        <v>40</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K25" s="1">
-        <v>32</v>
-      </c>
-      <c r="L25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="1">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="C26" s="1">
+        <v>26</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="K26" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L26" t="s">
-        <v>56</v>
-      </c>
-      <c r="M26" s="1">
-        <v>41</v>
-      </c>
-      <c r="N26" t="s">
-        <v>53</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="1">
+        <v>39</v>
+      </c>
+      <c r="K27" s="1">
+        <v>35</v>
+      </c>
+      <c r="L27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M27" s="1">
+        <v>41</v>
+      </c>
+      <c r="N27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B28" s="1">
         <v>37</v>
       </c>
-      <c r="K27" s="1">
+      <c r="C28" s="1">
+        <v>53</v>
+      </c>
+      <c r="K28" s="1">
         <v>33</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L28" t="s">
         <v>59</v>
       </c>
-      <c r="M27" s="1">
+      <c r="M28" s="1">
         <v>49</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N28" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L28"/>
-      <c r="M28" s="1"/>
-    </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="1">
-        <v>32</v>
-      </c>
-      <c r="K29" s="1">
-        <v>36</v>
-      </c>
-      <c r="L29" t="s">
-        <v>57</v>
-      </c>
-      <c r="M29" s="1">
-        <v>40</v>
-      </c>
-      <c r="N29" t="s">
-        <v>52</v>
-      </c>
+      <c r="L29"/>
+      <c r="M29" s="1"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="1">
-        <v>35</v>
-      </c>
-      <c r="C30" s="1">
-        <v>41</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="K30" s="1">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L30" t="s">
-        <v>58</v>
-      </c>
-      <c r="M30" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="M30" s="1">
+        <v>40</v>
+      </c>
+      <c r="N30" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="1">
+        <v>35</v>
+      </c>
+      <c r="C31" s="1">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K31" s="1">
+        <v>39</v>
+      </c>
+      <c r="L31" t="s">
+        <v>58</v>
+      </c>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B32" s="1">
         <v>33</v>
       </c>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1">
+      <c r="C32" s="1">
+        <v>49</v>
+      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1">
         <v>37</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L32" t="s">
         <v>59</v>
       </c>
-      <c r="M31" s="1">
+      <c r="M32" s="1">
         <v>53</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N32" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="1">
-        <v>64</v>
-      </c>
-      <c r="K34" s="1">
-        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K35" s="1">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K36" s="1">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1">
+        <v>66</v>
+      </c>
+      <c r="K37" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B38" s="1">
         <v>67</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K38" s="1">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed issues with how pages are displayed if top and bottom rows are linked showing racks/variations/songs/sonparts
</commit_message>
<xml_diff>
--- a/Preset CCs.xlsx
+++ b/Preset CCs.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Repos\GP-MC8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A5B6C3-990D-412E-A8D7-5238E129E7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C97E059-04ED-4C1E-A4DA-027C5084C88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30960" yWindow="2175" windowWidth="20445" windowHeight="12825" xr2:uid="{0B747C49-F5AE-45D7-856A-0899A5ED985A}"/>
+    <workbookView xWindow="330" yWindow="510" windowWidth="28410" windowHeight="14940" activeTab="1" xr2:uid="{0B747C49-F5AE-45D7-856A-0899A5ED985A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
   <si>
     <t>A</t>
   </si>
@@ -152,9 +153,6 @@
     <t>Exp 4</t>
   </si>
   <si>
-    <t>Coding of CCs</t>
-  </si>
-  <si>
     <t>bit 3</t>
   </si>
   <si>
@@ -249,6 +247,105 @@
   </si>
   <si>
     <t>Top</t>
+  </si>
+  <si>
+    <t>page back</t>
+  </si>
+  <si>
+    <t>page fwd</t>
+  </si>
+  <si>
+    <t>cycle display</t>
+  </si>
+  <si>
+    <t>Coding of CCs/notes</t>
+  </si>
+  <si>
+    <t>Button select</t>
+  </si>
+  <si>
+    <t>0 - 3</t>
+  </si>
+  <si>
+    <t>bottom buttons</t>
+  </si>
+  <si>
+    <t>4 - 7</t>
+  </si>
+  <si>
+    <t>top buttons</t>
+  </si>
+  <si>
+    <t>8 - 11</t>
+  </si>
+  <si>
+    <t>page two bottom buttons</t>
+  </si>
+  <si>
+    <t>12 - 15</t>
+  </si>
+  <si>
+    <t>page two top buttons</t>
+  </si>
+  <si>
+    <t>The MC8 Pro has 8 buttons that the MC replicates three time as</t>
+  </si>
+  <si>
+    <t>three "pages".  These correspond to presets A-H, I-P, and Q-X.</t>
+  </si>
+  <si>
+    <t>The Omniports can also accept TRS switches or a Resistor Ladder switch (only on Omniport 1).</t>
+  </si>
+  <si>
+    <t>These aux switches can be mapped to functions or presets, but not set to simply send a specific midi even</t>
+  </si>
+  <si>
+    <t>The MC6 Pro has 6 buttons that the MC will map to 4 pages, resulting in the same 24 total mapped buttons</t>
+  </si>
+  <si>
+    <t>as the MC8 and MC8 Pro</t>
+  </si>
+  <si>
+    <t>The aux and Ladder buttons can also be set to map to a specific preset (A-X), flip to a specific page (1-4), or</t>
+  </si>
+  <si>
+    <t>do other MC things, but also cannot simply send a predefined midi event</t>
+  </si>
+  <si>
+    <t>A feature and limitation of this model is that we can't fully utilize all "pages" of the display and make use of the</t>
+  </si>
+  <si>
+    <t>Aux/Ladder additional button functionality at the same time</t>
+  </si>
+  <si>
+    <t>Bottom row functions</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Cycle what is shown</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Top row functions</t>
+  </si>
+  <si>
+    <t>Generally assigned to Aux 1 TRS buttons</t>
+  </si>
+  <si>
+    <t>Generally assigned to Aux 2 TRS buttons</t>
+  </si>
+  <si>
+    <t>or to long-press of bottom row buttons</t>
+  </si>
+  <si>
+    <t>or to long-press of top row buttons</t>
+  </si>
+  <si>
+    <t>To simultaneously link top &amp; bottom row and page forward or back</t>
   </si>
 </sst>
 </file>
@@ -296,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,6 +412,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -333,9 +432,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -373,7 +472,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -479,7 +578,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -621,7 +720,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -631,11 +730,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159D800F-0466-47B0-AEE7-B390993F0385}">
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,13 +750,13 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1">
         <v>5</v>
@@ -665,7 +764,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -674,7 +773,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="4"/>
       <c r="J2" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
@@ -694,10 +793,10 @@
         <v>26</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J3" t="s">
         <v>2</v>
@@ -709,10 +808,10 @@
         <v>19</v>
       </c>
       <c r="M3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P3" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -744,10 +843,10 @@
         <v>16</v>
       </c>
       <c r="P4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" t="s">
         <v>41</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -779,10 +878,10 @@
         <v>17</v>
       </c>
       <c r="P5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -814,10 +913,10 @@
         <v>19</v>
       </c>
       <c r="P6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q6" t="s">
         <v>39</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -840,16 +939,16 @@
         <v>35</v>
       </c>
       <c r="P7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F8"/>
       <c r="P8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -881,7 +980,7 @@
         <v>20</v>
       </c>
       <c r="P9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -913,7 +1012,7 @@
         <v>21</v>
       </c>
       <c r="P10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -942,7 +1041,7 @@
         <v>23</v>
       </c>
       <c r="P11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -997,10 +1096,10 @@
         <v>24</v>
       </c>
       <c r="P14" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q14" t="s">
         <v>49</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1188,7 +1287,7 @@
         <v>47</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
@@ -1205,7 +1304,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -1222,13 +1321,16 @@
         <v>30</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>70</v>
       </c>
       <c r="K26" s="1">
         <v>32</v>
       </c>
       <c r="L26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N26" s="1"/>
     </row>
@@ -1239,17 +1341,20 @@
       <c r="B27" s="1">
         <v>39</v>
       </c>
+      <c r="G27" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="K27" s="1">
         <v>35</v>
       </c>
       <c r="L27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M27" s="1">
         <v>41</v>
       </c>
       <c r="N27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -1262,17 +1367,20 @@
       <c r="C28" s="1">
         <v>53</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="K28" s="1">
         <v>33</v>
       </c>
       <c r="L28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M28" s="1">
         <v>49</v>
       </c>
       <c r="N28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -1287,19 +1395,22 @@
         <v>32</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="K30" s="1">
         <v>36</v>
       </c>
       <c r="L30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M30" s="1">
         <v>40</v>
       </c>
       <c r="N30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -1315,11 +1426,14 @@
       <c r="D31" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="G31" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="K31" s="1">
         <v>39</v>
       </c>
       <c r="L31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M31" s="1"/>
     </row>
@@ -1333,18 +1447,21 @@
       <c r="C32" s="1">
         <v>49</v>
       </c>
+      <c r="G32" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1">
         <v>37</v>
       </c>
       <c r="L32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M32" s="1">
         <v>53</v>
       </c>
       <c r="N32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1389,6 +1506,178 @@
       </c>
       <c r="K38" s="1">
         <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D34A4B-34BC-45FE-B33F-F807E417BEE0}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="F4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mcx_d display widget stuff
</commit_message>
<xml_diff>
--- a/Preset CCs.xlsx
+++ b/Preset CCs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Repos\GP-MC8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C97E059-04ED-4C1E-A4DA-027C5084C88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1105399-B5E8-4D08-99DC-EF4239156164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="510" windowWidth="28410" windowHeight="14940" activeTab="1" xr2:uid="{0B747C49-F5AE-45D7-856A-0899A5ED985A}"/>
+    <workbookView xWindow="5490" yWindow="600" windowWidth="21390" windowHeight="14640" xr2:uid="{0B747C49-F5AE-45D7-856A-0899A5ED985A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="111">
   <si>
     <t>A</t>
   </si>
@@ -346,6 +346,30 @@
   </si>
   <si>
     <t>To simultaneously link top &amp; bottom row and page forward or back</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>0x23</t>
+  </si>
+  <si>
+    <t>thisaction</t>
+  </si>
+  <si>
+    <t>0x2</t>
+  </si>
+  <si>
+    <t>thisrow</t>
+  </si>
+  <si>
+    <t>thisposition</t>
+  </si>
+  <si>
+    <t>0x24</t>
+  </si>
+  <si>
+    <t>0x27</t>
   </si>
 </sst>
 </file>
@@ -730,11 +754,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159D800F-0466-47B0-AEE7-B390993F0385}">
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q18" sqref="Q18"/>
+      <selection pane="bottomRight" activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,6 +1330,15 @@
       <c r="A25" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="R25" t="s">
+        <v>105</v>
+      </c>
+      <c r="S25" t="s">
+        <v>107</v>
+      </c>
+      <c r="T25" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1333,13 +1366,25 @@
         <v>54</v>
       </c>
       <c r="N26" s="1"/>
+      <c r="Q26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="R26" t="s">
+        <v>106</v>
+      </c>
+      <c r="S26" s="2">
+        <v>0</v>
+      </c>
+      <c r="T26" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>72</v>
@@ -1355,6 +1400,18 @@
       </c>
       <c r="N27" t="s">
         <v>52</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>104</v>
+      </c>
+      <c r="R27" t="s">
+        <v>106</v>
+      </c>
+      <c r="S27" s="2">
+        <v>0</v>
+      </c>
+      <c r="T27" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -1362,7 +1419,7 @@
         <v>22</v>
       </c>
       <c r="B28" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C28" s="1">
         <v>53</v>
@@ -1412,13 +1469,25 @@
       <c r="N30" t="s">
         <v>51</v>
       </c>
+      <c r="Q30" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="R30" t="s">
+        <v>106</v>
+      </c>
+      <c r="S30" s="2">
+        <v>1</v>
+      </c>
+      <c r="T30" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
       <c r="B31" s="1">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" s="1">
         <v>18</v>
@@ -1436,13 +1505,25 @@
         <v>57</v>
       </c>
       <c r="M31" s="1"/>
+      <c r="Q31" t="s">
+        <v>110</v>
+      </c>
+      <c r="R31" t="s">
+        <v>106</v>
+      </c>
+      <c r="S31" s="2">
+        <v>1</v>
+      </c>
+      <c r="T31" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
       <c r="B32" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C32" s="1">
         <v>49</v>
@@ -1517,7 +1598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D34A4B-34BC-45FE-B33F-F807E417BEE0}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updates and minor display hiccup fixes, added [nextsong] [prevsong] special caption names, still WIP
</commit_message>
<xml_diff>
--- a/Preset CCs.xlsx
+++ b/Preset CCs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Repos\GP-MC8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1105399-B5E8-4D08-99DC-EF4239156164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E39294-FB98-42F2-A5F5-48A04AA06A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="600" windowWidth="21390" windowHeight="14640" xr2:uid="{0B747C49-F5AE-45D7-856A-0899A5ED985A}"/>
+    <workbookView xWindow="15240" yWindow="456" windowWidth="22836" windowHeight="16104" activeTab="1" xr2:uid="{0B747C49-F5AE-45D7-856A-0899A5ED985A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="125">
   <si>
     <t>A</t>
   </si>
@@ -370,14 +371,73 @@
   </si>
   <si>
     <t>0x27</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>button</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>whatever</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>Long Press</t>
+  </si>
+  <si>
+    <t>Goto page 2</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Goto page 1</t>
+  </si>
+  <si>
+    <t>Select &amp; set both rows</t>
+  </si>
+  <si>
+    <t>count = 19</t>
+  </si>
+  <si>
+    <t>current = 18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -417,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -438,6 +498,13 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,25 +821,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159D800F-0466-47B0-AEE7-B390993F0385}">
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U16" sqref="U16"/>
+      <selection pane="bottomRight" activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="11.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="11.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="2.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="10.33203125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>66</v>
       </c>
@@ -786,7 +853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>64</v>
       </c>
@@ -803,7 +870,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -838,7 +905,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -873,7 +940,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -908,7 +975,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -943,7 +1010,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -966,7 +1033,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="F8"/>
       <c r="P8" t="s">
         <v>60</v>
@@ -975,7 +1042,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1007,7 +1074,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1039,7 +1106,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1068,7 +1135,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1088,10 +1155,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1126,7 +1193,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1155,7 +1222,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1184,7 +1251,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1204,10 +1271,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F18"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1236,7 +1303,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1265,7 +1332,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1291,7 +1358,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1318,7 +1385,7 @@
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="J24" t="s">
         <v>32</v>
       </c>
@@ -1326,7 +1393,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>61</v>
       </c>
@@ -1340,7 +1407,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1379,7 +1446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1414,7 +1481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1440,11 +1507,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L29"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1482,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -1518,7 +1585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -1545,7 +1612,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1555,8 +1622,14 @@
       <c r="K35" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R35" t="s">
+        <v>123</v>
+      </c>
+      <c r="S35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1566,8 +1639,11 @@
       <c r="K36" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1578,7 +1654,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1595,6 +1671,494 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A11672-9A18-492A-81B0-E57094260168}">
+  <dimension ref="A2:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="2.5546875" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
+        <v>48</v>
+      </c>
+      <c r="I4" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>49</v>
+      </c>
+      <c r="I5" s="1">
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1">
+        <v>50</v>
+      </c>
+      <c r="I6" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
+        <v>51</v>
+      </c>
+      <c r="I7" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <v>52</v>
+      </c>
+      <c r="I9" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>53</v>
+      </c>
+      <c r="I10" s="1">
+        <v>37</v>
+      </c>
+      <c r="J10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1">
+        <v>54</v>
+      </c>
+      <c r="I11" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
+        <v>23</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
+        <v>55</v>
+      </c>
+      <c r="I12" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1">
+        <v>24</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1">
+        <v>56</v>
+      </c>
+      <c r="I15" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1">
+        <v>25</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1">
+        <v>57</v>
+      </c>
+      <c r="I16" s="1">
+        <v>41</v>
+      </c>
+      <c r="J16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1">
+        <v>26</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1">
+        <v>58</v>
+      </c>
+      <c r="I17" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1">
+        <v>27</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1">
+        <v>59</v>
+      </c>
+      <c r="I18" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1">
+        <v>28</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1">
+        <v>60</v>
+      </c>
+      <c r="I20" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1">
+        <v>13</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1">
+        <v>29</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1">
+        <v>61</v>
+      </c>
+      <c r="I21" s="1">
+        <v>45</v>
+      </c>
+      <c r="J21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1">
+        <v>14</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1">
+        <v>30</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1">
+        <v>62</v>
+      </c>
+      <c r="I22" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="1">
+        <v>15</v>
+      </c>
+      <c r="E23" s="1">
+        <v>31</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="1">
+        <v>63</v>
+      </c>
+      <c r="I23" s="1">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D34A4B-34BC-45FE-B33F-F807E417BEE0}">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -1602,9 +2166,9 @@
       <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -1612,7 +2176,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -1623,7 +2187,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>77</v>
       </c>
@@ -1634,13 +2198,13 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="F4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>79</v>
       </c>
@@ -1648,7 +2212,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>81</v>
       </c>
@@ -1659,17 +2223,17 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -1677,7 +2241,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>32</v>
       </c>
@@ -1685,7 +2249,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>35</v>
       </c>
@@ -1696,7 +2260,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>33</v>
       </c>
@@ -1707,22 +2271,22 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>36</v>
       </c>
@@ -1730,7 +2294,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>39</v>
       </c>
@@ -1738,7 +2302,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>37</v>
       </c>
@@ -1746,17 +2310,17 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>102</v>
       </c>

</xml_diff>